<commit_message>
Added ExtentReports code for reporting modules
</commit_message>
<xml_diff>
--- a/Excel_Data/LogIn_Data.xlsx
+++ b/Excel_Data/LogIn_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA_Testing_Doc\Keyword_Driven_Framework_For_ACA\Keyword_Driven_Framework_For_ACA\Excel_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA_Testing_Doc\Keyword_Driven_Framework_For_ACA\Keyword_Driven_Framework_For_ACA_With_Repository\Excel_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DD1E0E-8493-4E55-9676-3637BBD0C516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5565B56-99E9-4F9F-B991-BAA36C3144DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>TC_1</t>
   </si>
@@ -80,7 +80,10 @@
     <t>https://activate.mma.com/internal/launchpad/</t>
   </si>
   <si>
-    <t>Wolverine ACA Merrell LS</t>
+    <t>Abbott</t>
+  </si>
+  <si>
+    <t>DTC</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -548,7 +551,9 @@
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>